<commit_message>
erstellte Teil 1 des IPA Berichts ohne Arbeitsjournal
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -732,15 +732,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>5112</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>7567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>348343</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -750,7 +750,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10520712" y="5846392"/>
+          <a:off x="10520712" y="7827592"/>
           <a:ext cx="343231" cy="112176"/>
         </a:xfrm>
         <a:prstGeom prst="homePlate">
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR12" sqref="AR12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z84" sqref="Z84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Zeitplan für 24.03 Angepasst
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -978,15 +978,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>11395</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>8124</xdr:rowOff>
+      <xdr:colOff>3113</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>124080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>4500</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352370</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>120871</xdr:rowOff>
+      <xdr:rowOff>112588</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -995,8 +995,73 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5593045" y="2922774"/>
-          <a:ext cx="345530" cy="112747"/>
+          <a:off x="5610439" y="2931884"/>
+          <a:ext cx="349257" cy="112747"/>
+        </a:xfrm>
+        <a:prstGeom prst="homePlate">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>18850</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11955</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>120042</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Richtungspfeil 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5982328" y="3601947"/>
+          <a:ext cx="349257" cy="112747"/>
         </a:xfrm>
         <a:prstGeom prst="homePlate">
           <a:avLst/>
@@ -1311,7 +1376,9 @@
   </sheetPr>
   <dimension ref="A1:AR79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL29" sqref="AL29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2473,7 +2540,7 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+      <c r="I26" s="14"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>

</xml_diff>